<commit_message>
Se genera algoritmo quickSort y metricas
</commit_message>
<xml_diff>
--- a/Ordenamiento/Metricas.xlsx
+++ b/Ordenamiento/Metricas.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cambio Residuo" sheetId="1" r:id="rId1"/>
+    <sheet name="QuickSort" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -90,7 +91,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -101,6 +102,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -186,7 +188,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$51</c:f>
+              <c:f>'Cambio Residuo'!$B$2:$B$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -582,7 +584,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$L$2:$L$51</c:f>
+              <c:f>'Cambio Residuo'!$L$2:$L$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -910,6 +912,402 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>QuickSort!$A$1:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2.9999999999999999E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9999999999999997E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9999999999999996E-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2000000000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6000000000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.4000000000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.0999999999999997E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.4000000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.8999999999999997E-6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.6999999999999996E-6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.1E-6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.7000000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.9E-6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.7000000000000008E-6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.7000000000000008E-6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.1999999999999994E-6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.0999999999999993E-6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.3999999999999998E-6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.01E-5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.08E-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.1600000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.2099999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.2099999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.33E-5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.3699999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.38E-5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.5E-5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.7499999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.9300000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.9400000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.1299999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.6799999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.7600000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.84E-5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.8600000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.8499999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.0299999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.1999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.0999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.19E-5</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.2799999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.2900000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.34E-5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.3499999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.4600000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.44E-5</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.5599999999999999E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B293-4C87-87A3-5D1DA313AB59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="698316720"/>
+        <c:axId val="698322128"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="698316720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="698322128"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="698322128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="698316720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -990,6 +1388,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1507,6 +1945,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2079,6 +3033,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2352,7 +3341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
@@ -3178,4 +4167,273 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4">
+        <v>2.9999999999999999E-7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>6.9999999999999997E-7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>7.9999999999999996E-7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1.3E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>2.2000000000000001E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>2.6000000000000001E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>3.1E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>3.4000000000000001E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>4.0999999999999997E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>4.4000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>4.8999999999999997E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>5.6999999999999996E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>6.1E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>6.7000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>6.9E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>7.7000000000000008E-6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>7.7000000000000008E-6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>8.1999999999999994E-6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>9.0999999999999993E-6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>9.3999999999999998E-6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>1.01E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>1.08E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>1.1600000000000001E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>1.2099999999999999E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>1.2099999999999999E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>1.33E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>1.3699999999999999E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>1.38E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>1.5E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>1.7499999999999998E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>1.9300000000000002E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>1.9400000000000001E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>2.1299999999999999E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>1.6799999999999998E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>1.7600000000000001E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>1.84E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>1.8600000000000001E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>1.8499999999999999E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>2.0299999999999999E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>2.1999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>2.0999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>2.19E-5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>2.2799999999999999E-5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>2.2900000000000001E-5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>2.34E-5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>2.3499999999999999E-5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>2.4600000000000002E-5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>2.44E-5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>2.5599999999999999E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se realizan metricas y cambios en el comentado del codigo
</commit_message>
<xml_diff>
--- a/Ordenamiento/Metricas.xlsx
+++ b/Ordenamiento/Metricas.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cambio Residuo" sheetId="1" r:id="rId1"/>
     <sheet name="QuickSort" sheetId="2" r:id="rId2"/>
+    <sheet name="MergeSort" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -91,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -103,6 +104,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -135,7 +137,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -531,7 +532,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1308,6 +1308,402 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>MergeSort!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>7.9999999999999996E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0999999999999998E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0999999999999997E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.3999999999999997E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.2000000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.9000000000000003E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.7000000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.4000000000000003E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.7999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.6999999999999997E-6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.3000000000000007E-6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.01E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0699999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.17E-5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.27E-5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.3900000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.4600000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.5699999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.6399999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.6699999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.7900000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.8199999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.9199999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.98E-5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.05E-5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.09E-5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.6599999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.8600000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.1199999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.6100000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.8900000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.9799999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.0800000000000003E-5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.9E-5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.2499999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.1099999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.7499999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.2499999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.3000000000000003E-5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.3800000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.4499999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.4900000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.6000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.6300000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3.79E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7AA4-421F-93F1-3FF1029F0FC4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="483930576"/>
+        <c:axId val="483918928"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="483930576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="483918928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="483918928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="483930576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1428,6 +1824,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2461,6 +2897,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3055,6 +4007,41 @@
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4173,7 +5160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -4436,4 +5423,270 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>7.9999999999999996E-7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>1.3E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>2.0999999999999998E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>2.7E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>3.4999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>4.0999999999999997E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>6.3999999999999997E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>5.2000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>5.9000000000000003E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>6.7000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>7.4000000000000003E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>7.7999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>8.6999999999999997E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>9.3000000000000007E-6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>1.01E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>1.0699999999999999E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>1.17E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>1.24E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>1.27E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>1.3900000000000001E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>1.4600000000000001E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>1.5699999999999999E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>1.6399999999999999E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>1.6699999999999999E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>1.7900000000000001E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>1.8199999999999999E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>1.9199999999999999E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>1.98E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>2.05E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>2.09E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>2.6599999999999999E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>2.8600000000000001E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>3.1199999999999999E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>3.26E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>2.6100000000000001E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>2.8900000000000001E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>2.9799999999999999E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>3.0800000000000003E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>2.9E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>3.2499999999999997E-5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>3.1099999999999997E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>3.7499999999999997E-5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>3.2499999999999997E-5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>3.3000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>3.3800000000000002E-5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>3.4499999999999998E-5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <v>3.4900000000000001E-5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <v>3.6000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
+        <v>3.6300000000000001E-5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
+        <v>3.79E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega algoritmo de ordenamiento por base, y metricas
</commit_message>
<xml_diff>
--- a/Ordenamiento/Metricas.xlsx
+++ b/Ordenamiento/Metricas.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Cambio Residuo" sheetId="1" r:id="rId1"/>
     <sheet name="QuickSort" sheetId="2" r:id="rId2"/>
     <sheet name="MergeSort" sheetId="3" r:id="rId3"/>
     <sheet name="Base" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja2" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="6">
   <si>
     <t>1ra toma</t>
   </si>
@@ -46,13 +47,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -102,7 +108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -115,6 +121,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2789,6 +2799,1194 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1365878592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Base!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>4.9999999999999998E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.9000000000000003E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1999999999999994E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.03E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3900000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5699999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.48E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.7900000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.54E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.2200000000000003E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.9799999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.8799999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.69E-5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.2399999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.1000000000000004E-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.6700000000000007E-5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.2899999999999995E-5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.103E-4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.2520000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.3359999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.6640000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.627E-4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.6890000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.819E-4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.9780000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.14E-4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.2489999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.319E-4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.1119999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.7910000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.8739999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.7669999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.367E-4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.3149999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.5879999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.592E-4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.8200000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.1120000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.2620000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.793E-4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.9490000000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.176E-4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.373E-4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5.6090000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.7649999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>6.0409999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>6.5010000000000003E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5BC5-43E3-B7B9-13B37C055FAA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1120253535"/>
+        <c:axId val="1120254783"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1120253535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1120254783"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1120254783"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1120253535"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Base!$J$2:$J$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.301029995663981</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.477121254719663</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.602059991327963</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51.698970004336019</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61.778151250383644</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>71.84509804001425</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>81.903089986991944</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>91.954242509439325</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>112.04139268515823</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>122.07918124604763</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>132.11394335230685</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>142.14612803567823</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>152.17609125905568</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>162.20411998265593</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>172.23044892137827</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>182.25527250510331</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>192.27875360095283</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>202.30102999566398</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>212.32221929473391</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>222.34242268082221</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>232.36172783601759</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>242.38021124171161</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>252.39794000867204</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>262.41497334797083</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>272.43136376415896</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>282.44715803134221</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>292.46239799789896</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>302.47712125471969</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>312.49136169383428</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>322.50514997831988</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>332.51851393987789</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>342.53147891704225</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>352.5440680443503</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>362.55630250076729</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>372.56820172406697</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>382.57978359661683</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>392.59106460702651</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>402.60205999132796</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>412.61278385671972</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>422.62324929039789</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>432.63346845557959</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>442.64345267648616</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>452.65321251377532</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>462.66275783168157</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>472.67209785793574</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>482.68124123737556</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>492.6901960800285</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>502.69897000433605</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6D94-4B59-8A48-B9B39FEF8DAB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1120247295"/>
+        <c:axId val="1120251039"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1120247295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1120251039"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1120251039"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1120247295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$A$1:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>7.9999999999999996E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5000000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.9000000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.4000000000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.8999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.3000000000000003E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.9999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.7000000000000008E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.3999999999999992E-6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.0999999999999993E-6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.7000000000000003E-6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.04E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.1E-5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.1800000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.24E-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.31E-5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.3699999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.4399999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.5099999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.5999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.6500000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.7200000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.7799999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.8499999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.1399999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.9899999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.0599999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.69E-5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.1999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.27E-5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.3200000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.4000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.4700000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.5299999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.6100000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.15E-5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.4400000000000003E-5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.8099999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.9099999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.6900000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.0300000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.0800000000000003E-5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.1399999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.2100000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.2799999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.3399999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3.43E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B38-4D0D-B16E-E97570777018}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1059138591"/>
+        <c:axId val="1059134431"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1059138591"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1059134431"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1059134431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1059138591"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3077,6 +4275,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -5658,6 +6976,1554 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6368,6 +9234,106 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -6633,7 +9599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
@@ -7521,7 +10487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
   </sheetViews>
@@ -8205,8 +11171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8885,20 +11851,948 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
+      </c>
+      <c r="I2" s="2">
+        <v>10</v>
+      </c>
+      <c r="J2" s="3">
+        <f>I2+LOG10(I2)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1.3999999999999999E-6</v>
+      </c>
+      <c r="I3" s="2">
+        <f>I2+10</f>
+        <v>20</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" ref="J3:J51" si="0">I3+LOG10(I3)</f>
+        <v>21.301029995663981</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2.3999999999999999E-6</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" ref="I4:I51" si="1">I3+10</f>
+        <v>30</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="0"/>
+        <v>31.477121254719663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>3.8E-6</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="0"/>
+        <v>41.602059991327963</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5.9000000000000003E-6</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="0"/>
+        <v>51.698970004336019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>8.1999999999999994E-6</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="0"/>
+        <v>61.778151250383644</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>1.03E-5</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="0"/>
+        <v>71.84509804001425</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>1.3900000000000001E-5</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="0"/>
+        <v>81.903089986991944</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>1.5699999999999999E-5</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="0"/>
+        <v>91.954242509439325</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>2.48E-5</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="0"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>2.7900000000000001E-5</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="0"/>
+        <v>112.04139268515823</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>3.54E-5</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="0"/>
+        <v>122.07918124604763</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>4.2200000000000003E-5</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="0"/>
+        <v>132.11394335230685</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>4.9799999999999998E-5</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="0"/>
+        <v>142.14612803567823</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>5.8799999999999999E-5</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="0"/>
+        <v>152.17609125905568</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>6.69E-5</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" si="0"/>
+        <v>162.20411998265593</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>7.2399999999999998E-5</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="1"/>
+        <v>170</v>
+      </c>
+      <c r="J18" s="3">
+        <f t="shared" si="0"/>
+        <v>172.23044892137827</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>8.1000000000000004E-5</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+      <c r="J19" s="3">
+        <f t="shared" si="0"/>
+        <v>182.25527250510331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>8.6700000000000007E-5</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="1"/>
+        <v>190</v>
+      </c>
+      <c r="J20" s="3">
+        <f t="shared" si="0"/>
+        <v>192.27875360095283</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>9.2899999999999995E-5</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="J21" s="3">
+        <f t="shared" si="0"/>
+        <v>202.30102999566398</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>1.103E-4</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
+      <c r="J22" s="3">
+        <f t="shared" si="0"/>
+        <v>212.32221929473391</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>1.2520000000000001E-4</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
+      <c r="J23" s="3">
+        <f t="shared" si="0"/>
+        <v>222.34242268082221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>1.3359999999999999E-4</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="1"/>
+        <v>230</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="0"/>
+        <v>232.36172783601759</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>1.6640000000000001E-4</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="J25" s="3">
+        <f t="shared" si="0"/>
+        <v>242.38021124171161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>1.627E-4</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="J26" s="3">
+        <f t="shared" si="0"/>
+        <v>252.39794000867204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>1.6890000000000001E-4</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="1"/>
+        <v>260</v>
+      </c>
+      <c r="J27" s="3">
+        <f t="shared" si="0"/>
+        <v>262.41497334797083</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>1.819E-4</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="1"/>
+        <v>270</v>
+      </c>
+      <c r="J28" s="3">
+        <f t="shared" si="0"/>
+        <v>272.43136376415896</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>1.9780000000000001E-4</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="1"/>
+        <v>280</v>
+      </c>
+      <c r="J29" s="3">
+        <f t="shared" si="0"/>
+        <v>282.44715803134221</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>2.14E-4</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="1"/>
+        <v>290</v>
+      </c>
+      <c r="J30" s="3">
+        <f t="shared" si="0"/>
+        <v>292.46239799789896</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>2.2489999999999999E-4</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="J31" s="3">
+        <f t="shared" si="0"/>
+        <v>302.47712125471969</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>2.319E-4</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="1"/>
+        <v>310</v>
+      </c>
+      <c r="J32" s="3">
+        <f t="shared" si="0"/>
+        <v>312.49136169383428</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>3.1119999999999997E-4</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="1"/>
+        <v>320</v>
+      </c>
+      <c r="J33" s="3">
+        <f t="shared" si="0"/>
+        <v>322.50514997831988</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>2.7910000000000001E-4</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="1"/>
+        <v>330</v>
+      </c>
+      <c r="J34" s="3">
+        <f t="shared" si="0"/>
+        <v>332.51851393987789</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>2.8739999999999999E-4</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="1"/>
+        <v>340</v>
+      </c>
+      <c r="J35" s="3">
+        <f t="shared" si="0"/>
+        <v>342.53147891704225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>3.7669999999999999E-4</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="1"/>
+        <v>350</v>
+      </c>
+      <c r="J36" s="3">
+        <f t="shared" si="0"/>
+        <v>352.5440680443503</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>3.367E-4</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+      <c r="J37" s="3">
+        <f t="shared" si="0"/>
+        <v>362.55630250076729</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>3.3149999999999998E-4</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="1"/>
+        <v>370</v>
+      </c>
+      <c r="J38" s="3">
+        <f t="shared" si="0"/>
+        <v>372.56820172406697</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>3.5879999999999999E-4</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="1"/>
+        <v>380</v>
+      </c>
+      <c r="J39" s="3">
+        <f t="shared" si="0"/>
+        <v>382.57978359661683</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>3.592E-4</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+      <c r="J40" s="3">
+        <f t="shared" si="0"/>
+        <v>392.59106460702651</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>3.8200000000000002E-4</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="J41" s="3">
+        <f t="shared" si="0"/>
+        <v>402.60205999132796</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>4.1120000000000002E-4</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="1"/>
+        <v>410</v>
+      </c>
+      <c r="J42" s="3">
+        <f t="shared" si="0"/>
+        <v>412.61278385671972</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>4.2620000000000001E-4</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+      <c r="J43" s="3">
+        <f t="shared" si="0"/>
+        <v>422.62324929039789</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>4.793E-4</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="1"/>
+        <v>430</v>
+      </c>
+      <c r="J44" s="3">
+        <f t="shared" si="0"/>
+        <v>432.63346845557959</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>4.9490000000000005E-4</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="1"/>
+        <v>440</v>
+      </c>
+      <c r="J45" s="3">
+        <f t="shared" si="0"/>
+        <v>442.64345267648616</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>5.176E-4</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="J46" s="3">
+        <f t="shared" si="0"/>
+        <v>452.65321251377532</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>5.373E-4</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="1"/>
+        <v>460</v>
+      </c>
+      <c r="J47" s="3">
+        <f t="shared" si="0"/>
+        <v>462.66275783168157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>5.6090000000000003E-4</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="1"/>
+        <v>470</v>
+      </c>
+      <c r="J48" s="3">
+        <f t="shared" si="0"/>
+        <v>472.67209785793574</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>5.7649999999999997E-4</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
+      <c r="J49" s="3">
+        <f t="shared" si="0"/>
+        <v>482.68124123737556</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>6.0409999999999999E-4</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="1"/>
+        <v>490</v>
+      </c>
+      <c r="J50" s="3">
+        <f t="shared" si="0"/>
+        <v>492.6901960800285</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>6.5010000000000003E-4</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="J51" s="3">
+        <f t="shared" si="0"/>
+        <v>502.69897000433605</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7">
+        <v>7.9999999999999996E-7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1.3E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>1.5999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>1.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>2.5000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>2.9000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>3.4000000000000001E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>3.8999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>4.3000000000000003E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>6.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>7.7000000000000008E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>8.3999999999999992E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>9.0999999999999993E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>9.7000000000000003E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>1.04E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>1.1E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>1.1800000000000001E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>1.24E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>1.31E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>1.3699999999999999E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>1.4399999999999999E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>1.5099999999999999E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>1.5999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>1.6500000000000001E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>1.7200000000000001E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>1.7799999999999999E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>1.8499999999999999E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>2.1399999999999998E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>1.9899999999999999E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>2.0599999999999999E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>2.69E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>2.1999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>2.27E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>2.3200000000000001E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>2.4000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>2.4700000000000001E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>2.5299999999999998E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <v>2.6100000000000001E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>3.15E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <v>3.4400000000000003E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>2.8099999999999999E-5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <v>2.9099999999999999E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>3.6900000000000002E-5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <v>3.0300000000000001E-5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <v>3.0800000000000003E-5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
+        <v>3.1399999999999998E-5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>3.2100000000000001E-5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <v>3.2799999999999998E-5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>3.3399999999999999E-5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>3.43E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se realiza cambio a comentarios
</commit_message>
<xml_diff>
--- a/Ordenamiento/Metricas.xlsx
+++ b/Ordenamiento/Metricas.xlsx
@@ -9304,15 +9304,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12533,7 +12533,7 @@
   <dimension ref="A1:A50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>